<commit_message>
phase 4 experiment data + all original data
</commit_message>
<xml_diff>
--- a/data/original/exercises/020-qualtrics/010-signin.xlsx
+++ b/data/original/exercises/020-qualtrics/010-signin.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1240,6 +1240,522 @@
         </is>
       </c>
     </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>44523.78958333333</v>
+      </c>
+      <c r="C21" s="2">
+        <v>44523.79026620371</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E21">
+        <v>100</v>
+      </c>
+      <c r="F21">
+        <v>58</v>
+      </c>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2">
+        <v>44523.79026620371</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>1pogus</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>44523.79092592593</v>
+      </c>
+      <c r="C22" s="2">
+        <v>44523.79208333333</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E22">
+        <v>100</v>
+      </c>
+      <c r="F22">
+        <v>99</v>
+      </c>
+      <c r="G22" t="b">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2">
+        <v>44523.79208333333</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>1dabec</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>44523.79164351852</v>
+      </c>
+      <c r="C23" s="2">
+        <v>44523.7924537037</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E23">
+        <v>100</v>
+      </c>
+      <c r="F23">
+        <v>70</v>
+      </c>
+      <c r="G23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H23" s="2">
+        <v>44523.7924537037</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>4lianj</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>44523.79159722223</v>
+      </c>
+      <c r="C24" s="2">
+        <v>44523.79251157407</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E24">
+        <v>100</v>
+      </c>
+      <c r="F24">
+        <v>78</v>
+      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" s="2">
+        <v>44523.79251157407</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>3hostc</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>44523.7925462963</v>
+      </c>
+      <c r="C25" s="2">
+        <v>44523.79327546296</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E25">
+        <v>100</v>
+      </c>
+      <c r="F25">
+        <v>63</v>
+      </c>
+      <c r="G25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H25" s="2">
+        <v>44523.79327546296</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>0LIBOL</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>44523.79273148148</v>
+      </c>
+      <c r="C26" s="2">
+        <v>44523.79327546296</v>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E26">
+        <v>100</v>
+      </c>
+      <c r="F26">
+        <v>47</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" s="2">
+        <v>44523.79328703704</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>1sawes</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>44523.79199074074</v>
+      </c>
+      <c r="C27" s="2">
+        <v>44523.79365740741</v>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>144</v>
+      </c>
+      <c r="G27" t="b">
+        <v>1</v>
+      </c>
+      <c r="H27" s="2">
+        <v>44523.79365740741</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2dunic</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>44523.7921412037</v>
+      </c>
+      <c r="C28" s="2">
+        <v>44523.79421296297</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E28">
+        <v>100</v>
+      </c>
+      <c r="F28">
+        <v>178</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" s="2">
+        <v>44523.79421296297</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>1bimil</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44523.79256944444</v>
+      </c>
+      <c r="C29" s="2">
+        <v>44523.79449074074</v>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E29">
+        <v>100</v>
+      </c>
+      <c r="F29">
+        <v>165</v>
+      </c>
+      <c r="G29" t="b">
+        <v>1</v>
+      </c>
+      <c r="H29" s="2">
+        <v>44523.79449074074</v>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>1lacat</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2">
+        <v>44523.79333333334</v>
+      </c>
+      <c r="C30" s="2">
+        <v>44523.79483796297</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+      <c r="F30">
+        <v>130</v>
+      </c>
+      <c r="G30" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="2">
+        <v>44523.79483796297</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>3mihar</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44523.7950462963</v>
+      </c>
+      <c r="C31" s="2">
+        <v>44523.79575231481</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+      <c r="F31">
+        <v>61</v>
+      </c>
+      <c r="G31" t="b">
+        <v>1</v>
+      </c>
+      <c r="H31" s="2">
+        <v>44523.79575231481</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2micar</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>44523.79260416667</v>
+      </c>
+      <c r="C32" s="2">
+        <v>44523.79762731482</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>IP Address</t>
+        </is>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+      <c r="F32">
+        <v>434</v>
+      </c>
+      <c r="G32" t="b">
+        <v>1</v>
+      </c>
+      <c r="H32" s="2">
+        <v>44523.79762731482</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Yes. I am 18 years of age or older.</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Yes. I have read the consent form and this response will serve as my consent to participate in the research study.</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>1davec</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>